<commit_message>
statistics for last release
</commit_message>
<xml_diff>
--- a/intenz-database/src/site/resources/statistics/intenzStats-2014.xlsx
+++ b/intenz-database/src/site/resources/statistics/intenzStats-2014.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="363" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="453" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="Table" sheetId="1" state="visible" r:id="rId2"/>
@@ -392,7 +392,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -452,10 +452,10 @@
                   <c:v>95</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v/>
+                  <c:v>96</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v/>
+                  <c:v>97</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v/>
@@ -494,10 +494,10 @@
                   <c:v>5292</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v/>
+                  <c:v>5292</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v/>
+                  <c:v>5383</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v/>
@@ -560,10 +560,10 @@
                   <c:v>95</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v/>
+                  <c:v>96</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v/>
+                  <c:v>97</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v/>
@@ -602,10 +602,10 @@
                   <c:v>869</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v/>
+                  <c:v>869</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v/>
+                  <c:v>877</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v/>
@@ -668,10 +668,10 @@
                   <c:v>95</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v/>
+                  <c:v>96</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v/>
+                  <c:v>97</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v/>
@@ -710,10 +710,10 @@
                   <c:v>68</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v/>
+                  <c:v>74</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v/>
+                  <c:v>61</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v/>
@@ -776,10 +776,10 @@
                   <c:v>95</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v/>
+                  <c:v>96</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v/>
+                  <c:v>97</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v/>
@@ -818,10 +818,10 @@
                   <c:v>134</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v/>
+                  <c:v>134</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v/>
+                  <c:v>148</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v/>
@@ -884,10 +884,10 @@
                   <c:v>95</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v/>
+                  <c:v>96</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v/>
+                  <c:v>97</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v/>
@@ -992,10 +992,10 @@
                   <c:v>95</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v/>
+                  <c:v>96</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v/>
+                  <c:v>97</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v/>
@@ -1100,10 +1100,10 @@
                   <c:v>95</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v/>
+                  <c:v>96</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v/>
+                  <c:v>97</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v/>
@@ -1208,10 +1208,10 @@
                   <c:v>95</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v/>
+                  <c:v>96</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v/>
+                  <c:v>97</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v/>
@@ -1285,11 +1285,11 @@
         </c:ser>
         <c:overlap val="100"/>
         <c:gapWidth val="100"/>
-        <c:axId val="67739552"/>
-        <c:axId val="45600531"/>
+        <c:axId val="33292058"/>
+        <c:axId val="22571829"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="67739552"/>
+        <c:axId val="33292058"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1323,14 +1323,14 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="45600531"/>
+        <c:crossAx val="22571829"/>
         <c:crossesAt val="3000"/>
         <c:lblAlgn val="ctr"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="45600531"/>
+        <c:axId val="22571829"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="3000"/>
@@ -1379,7 +1379,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="67739552"/>
+        <c:crossAx val="33292058"/>
         <c:crosses val="min"/>
       </c:valAx>
       <c:spPr>
@@ -1407,7 +1407,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -1467,10 +1467,10 @@
                   <c:v>95</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v/>
+                  <c:v>96</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v/>
+                  <c:v>97</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v/>
@@ -1509,10 +1509,10 @@
                   <c:v>6161</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>6161</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>6260</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
@@ -1575,10 +1575,10 @@
                   <c:v>95</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v/>
+                  <c:v>96</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v/>
+                  <c:v>97</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v/>
@@ -1617,10 +1617,10 @@
                   <c:v>202</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>208</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>209</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
@@ -1683,10 +1683,10 @@
                   <c:v>95</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v/>
+                  <c:v>96</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v/>
+                  <c:v>97</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v/>
@@ -1728,7 +1728,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>3988</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
@@ -1760,11 +1760,11 @@
         </c:ser>
         <c:overlap val="100"/>
         <c:gapWidth val="100"/>
-        <c:axId val="12343029"/>
-        <c:axId val="20934956"/>
+        <c:axId val="95700576"/>
+        <c:axId val="92498339"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="12343029"/>
+        <c:axId val="95700576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1798,17 +1798,17 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="20934956"/>
+        <c:crossAx val="92498339"/>
         <c:crossesAt val="0"/>
         <c:lblAlgn val="ctr"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="20934956"/>
+        <c:axId val="92498339"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:min val="4600"/>
+          <c:min val="3000"/>
         </c:scaling>
         <c:title>
           <c:layout/>
@@ -1854,10 +1854,10 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="12343029"/>
+        <c:crossAx val="95700576"/>
         <c:crosses val="min"/>
-        <c:majorUnit val="100"/>
-        <c:minorUnit val="50"/>
+        <c:majorUnit val="500"/>
+        <c:minorUnit val="250"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -1884,7 +1884,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -1944,10 +1944,10 @@
                   <c:v>95</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v/>
+                  <c:v>96</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v/>
+                  <c:v>97</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v/>
@@ -1986,10 +1986,10 @@
                   <c:v>3353</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v/>
+                  <c:v>3353</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v/>
+                  <c:v>3350</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v/>
@@ -2052,10 +2052,10 @@
                   <c:v>95</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v/>
+                  <c:v>96</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v/>
+                  <c:v>97</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v/>
@@ -2094,10 +2094,10 @@
                   <c:v>131</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v/>
+                  <c:v>132</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v/>
+                  <c:v>133</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v/>
@@ -2160,10 +2160,10 @@
                   <c:v>95</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v/>
+                  <c:v>96</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v/>
+                  <c:v>97</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v/>
@@ -2202,10 +2202,10 @@
                   <c:v>344</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v/>
+                  <c:v>344</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v/>
+                  <c:v>344</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v/>
@@ -2268,10 +2268,10 @@
                   <c:v>95</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v/>
+                  <c:v>96</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v/>
+                  <c:v>97</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v/>
@@ -2310,10 +2310,10 @@
                   <c:v>351</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v/>
+                  <c:v>351</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v/>
+                  <c:v>350</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v/>
@@ -2376,10 +2376,10 @@
                   <c:v>95</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v/>
+                  <c:v>96</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v/>
+                  <c:v>97</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v/>
@@ -2418,10 +2418,10 @@
                   <c:v>217</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v/>
+                  <c:v>217</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v/>
+                  <c:v>217</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v/>
@@ -2484,10 +2484,10 @@
                   <c:v>95</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v/>
+                  <c:v>96</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v/>
+                  <c:v>97</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v/>
@@ -2526,10 +2526,10 @@
                   <c:v>671</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v/>
+                  <c:v>670</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v/>
+                  <c:v>668</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v/>
@@ -2561,11 +2561,11 @@
         </c:ser>
         <c:overlap val="100"/>
         <c:gapWidth val="100"/>
-        <c:axId val="39161563"/>
-        <c:axId val="91980735"/>
+        <c:axId val="9211191"/>
+        <c:axId val="74735576"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="39161563"/>
+        <c:axId val="9211191"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2604,14 +2604,14 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="91980735"/>
+        <c:crossAx val="74735576"/>
         <c:crossesAt val="0"/>
         <c:lblAlgn val="ctr"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="91980735"/>
+        <c:axId val="74735576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2659,7 +2659,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="39161563"/>
+        <c:crossAx val="9211191"/>
         <c:crosses val="min"/>
       </c:valAx>
       <c:spPr>
@@ -2687,7 +2687,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -2747,10 +2747,10 @@
                   <c:v>95</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v/>
+                  <c:v>96</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v/>
+                  <c:v>97</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v/>
@@ -2789,10 +2789,10 @@
                   <c:v>212590</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v/>
+                  <c:v>212893</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v/>
+                  <c:v>212718</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v/>
@@ -2855,10 +2855,10 @@
                   <c:v>95</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v/>
+                  <c:v>96</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v/>
+                  <c:v>97</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v/>
@@ -2897,10 +2897,10 @@
                   <c:v>466</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v/>
+                  <c:v>466</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v/>
+                  <c:v>466</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v/>
@@ -2963,10 +2963,10 @@
                   <c:v>95</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v/>
+                  <c:v>96</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v/>
+                  <c:v>97</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v/>
@@ -3005,10 +3005,10 @@
                   <c:v>3958</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v/>
+                  <c:v>3959</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v/>
+                  <c:v>3959</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v/>
@@ -3071,10 +3071,10 @@
                   <c:v>95</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v/>
+                  <c:v>96</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v/>
+                  <c:v>97</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v/>
@@ -3113,10 +3113,10 @@
                   <c:v>573</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v/>
+                  <c:v>573</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v/>
+                  <c:v>573</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v/>
@@ -3148,11 +3148,11 @@
         </c:ser>
         <c:overlap val="100"/>
         <c:gapWidth val="100"/>
-        <c:axId val="20079750"/>
-        <c:axId val="33822515"/>
+        <c:axId val="92360204"/>
+        <c:axId val="39946026"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="20079750"/>
+        <c:axId val="92360204"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3168,14 +3168,14 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="33822515"/>
+        <c:crossAx val="39946026"/>
         <c:crossesAt val="0"/>
         <c:lblAlgn val="ctr"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="33822515"/>
+        <c:axId val="39946026"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="160000"/>
@@ -3224,7 +3224,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="20079750"/>
+        <c:crossAx val="92360204"/>
         <c:crosses val="min"/>
       </c:valAx>
       <c:spPr>
@@ -3252,7 +3252,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -3312,10 +3312,10 @@
                   <c:v>95</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v/>
+                  <c:v>96</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v/>
+                  <c:v>97</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v/>
@@ -3354,10 +3354,10 @@
                   <c:v>224132</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v/>
+                  <c:v>224460</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v/>
+                  <c:v>224291</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v/>
@@ -3420,10 +3420,10 @@
                   <c:v>95</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v/>
+                  <c:v>96</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v/>
+                  <c:v>97</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v/>
@@ -3462,10 +3462,10 @@
                   <c:v>1441</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v/>
+                  <c:v>1441</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v/>
+                  <c:v>1440</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v/>
@@ -3528,10 +3528,10 @@
                   <c:v>95</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v/>
+                  <c:v>96</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v/>
+                  <c:v>97</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v/>
@@ -3570,10 +3570,10 @@
                   <c:v>3987</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v/>
+                  <c:v>3988</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v/>
+                  <c:v>3988</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v/>
@@ -3636,10 +3636,10 @@
                   <c:v>95</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v/>
+                  <c:v>96</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v/>
+                  <c:v>97</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v/>
@@ -3678,10 +3678,10 @@
                   <c:v>1744</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v/>
+                  <c:v>1744</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v/>
+                  <c:v>1747</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v/>
@@ -3713,11 +3713,11 @@
         </c:ser>
         <c:overlap val="100"/>
         <c:gapWidth val="100"/>
-        <c:axId val="39631196"/>
-        <c:axId val="46162336"/>
+        <c:axId val="91548494"/>
+        <c:axId val="53736695"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="39631196"/>
+        <c:axId val="91548494"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3733,14 +3733,14 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="46162336"/>
+        <c:crossAx val="53736695"/>
         <c:crossesAt val="0"/>
         <c:lblAlgn val="ctr"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="46162336"/>
+        <c:axId val="53736695"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="160000"/>
@@ -3789,7 +3789,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="39631196"/>
+        <c:crossAx val="91548494"/>
         <c:crosses val="min"/>
       </c:valAx>
       <c:spPr>
@@ -3817,7 +3817,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -3851,10 +3851,10 @@
                   <c:v>95</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v/>
+                  <c:v>96</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v/>
+                  <c:v>97</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v/>
@@ -3893,10 +3893,10 @@
                   <c:v>20129</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v/>
+                  <c:v>20129</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v/>
+                  <c:v>20319</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v/>
@@ -3927,11 +3927,11 @@
           </c:val>
         </c:ser>
         <c:marker val="0"/>
-        <c:axId val="10160007"/>
-        <c:axId val="41616912"/>
+        <c:axId val="31180946"/>
+        <c:axId val="65128132"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="10160007"/>
+        <c:axId val="31180946"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3970,14 +3970,14 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="41616912"/>
+        <c:crossAx val="65128132"/>
         <c:crossesAt val="17000"/>
         <c:lblAlgn val="ctr"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="41616912"/>
+        <c:axId val="65128132"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -4026,7 +4026,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="10160007"/>
+        <c:crossAx val="31180946"/>
         <c:crosses val="min"/>
       </c:valAx>
       <c:spPr>
@@ -4052,7 +4052,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>165600</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>3960</xdr:rowOff>
+      <xdr:rowOff>4320</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
@@ -4066,8 +4066,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="165600" y="163080"/>
-        <a:ext cx="11599920" cy="3834000"/>
+        <a:off x="165600" y="163440"/>
+        <a:ext cx="11599920" cy="3833640"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4082,7 +4082,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>152280</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>90720</xdr:rowOff>
+      <xdr:rowOff>91080</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
@@ -4096,8 +4096,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="152280" y="4084560"/>
-        <a:ext cx="11638800" cy="3737880"/>
+        <a:off x="152280" y="4084920"/>
+        <a:ext cx="11638800" cy="3737520"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4182,7 +4182,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>318600</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>150120</xdr:rowOff>
+      <xdr:rowOff>150480</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
@@ -4196,8 +4196,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="318600" y="3846240"/>
-        <a:ext cx="11249640" cy="3766320"/>
+        <a:off x="318600" y="3846600"/>
+        <a:ext cx="11249640" cy="3765960"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4253,7 +4253,7 @@
   <dimension ref="A1:O45"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="B2" activeCellId="0" pane="topLeft" sqref="B2"/>
+      <selection activeCell="E1" activeCellId="0" pane="topLeft" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.1"/>
@@ -4269,6 +4269,12 @@
       <c r="B1" s="1" t="n">
         <v>95</v>
       </c>
+      <c r="C1" s="1" t="n">
+        <v>96</v>
+      </c>
+      <c r="D1" s="1" t="n">
+        <v>97</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="2">
       <c r="A2" s="1" t="s">
@@ -4277,8 +4283,12 @@
       <c r="B2" s="2" t="n">
         <v>41646</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
+      <c r="C2" s="2" t="n">
+        <v>41674</v>
+      </c>
+      <c r="D2" s="2" t="n">
+        <v>41704</v>
+      </c>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
@@ -4298,6 +4308,12 @@
       <c r="B3" s="0" t="n">
         <v>6</v>
       </c>
+      <c r="C3" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="4">
       <c r="A4" s="1" t="s">
@@ -4306,6 +4322,12 @@
       <c r="B4" s="0" t="n">
         <v>69</v>
       </c>
+      <c r="C4" s="0" t="n">
+        <v>69</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>69</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="5">
       <c r="A5" s="1" t="s">
@@ -4314,6 +4336,12 @@
       <c r="B5" s="0" t="n">
         <v>287</v>
       </c>
+      <c r="C5" s="0" t="n">
+        <v>287</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>287</v>
+      </c>
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
     </row>
@@ -4324,6 +4352,12 @@
       <c r="B6" s="4" t="n">
         <v>20129</v>
       </c>
+      <c r="C6" s="0" t="n">
+        <v>20129</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>20319</v>
+      </c>
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
     </row>
@@ -4342,6 +4376,12 @@
       <c r="B8" s="4" t="n">
         <v>5292</v>
       </c>
+      <c r="C8" s="0" t="n">
+        <v>5292</v>
+      </c>
+      <c r="D8" s="0" t="n">
+        <v>5383</v>
+      </c>
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
     </row>
@@ -4352,6 +4392,12 @@
       <c r="B9" s="4" t="n">
         <v>869</v>
       </c>
+      <c r="C9" s="0" t="n">
+        <v>869</v>
+      </c>
+      <c r="D9" s="0" t="n">
+        <v>877</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="10">
       <c r="A10" s="4" t="s">
@@ -4360,6 +4406,12 @@
       <c r="B10" s="4" t="n">
         <v>68</v>
       </c>
+      <c r="C10" s="0" t="n">
+        <v>74</v>
+      </c>
+      <c r="D10" s="0" t="n">
+        <v>61</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="11">
       <c r="A11" s="4" t="s">
@@ -4368,6 +4420,12 @@
       <c r="B11" s="4" t="n">
         <v>134</v>
       </c>
+      <c r="C11" s="0" t="n">
+        <v>134</v>
+      </c>
+      <c r="D11" s="0" t="n">
+        <v>148</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="12">
       <c r="A12" s="4" t="s">
@@ -4403,6 +4461,12 @@
       <c r="B17" s="0" t="n">
         <v>1744</v>
       </c>
+      <c r="C17" s="0" t="n">
+        <v>1744</v>
+      </c>
+      <c r="D17" s="0" t="n">
+        <v>1747</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="18">
       <c r="A18" s="4" t="s">
@@ -4411,6 +4475,12 @@
       <c r="B18" s="0" t="n">
         <v>3987</v>
       </c>
+      <c r="C18" s="0" t="n">
+        <v>3988</v>
+      </c>
+      <c r="D18" s="0" t="n">
+        <v>3988</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="19">
       <c r="A19" s="4" t="s">
@@ -4419,6 +4489,12 @@
       <c r="B19" s="0" t="n">
         <v>1441</v>
       </c>
+      <c r="C19" s="0" t="n">
+        <v>1441</v>
+      </c>
+      <c r="D19" s="0" t="n">
+        <v>1440</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="20">
       <c r="A20" s="4" t="s">
@@ -4427,6 +4503,12 @@
       <c r="B20" s="0" t="n">
         <v>224132</v>
       </c>
+      <c r="C20" s="0" t="n">
+        <v>224460</v>
+      </c>
+      <c r="D20" s="0" t="n">
+        <v>224291</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="21">
       <c r="A21" s="1" t="s">
@@ -4440,6 +4522,12 @@
       <c r="B22" s="0" t="n">
         <v>573</v>
       </c>
+      <c r="C22" s="0" t="n">
+        <v>573</v>
+      </c>
+      <c r="D22" s="0" t="n">
+        <v>573</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="23">
       <c r="A23" s="4" t="s">
@@ -4448,6 +4536,12 @@
       <c r="B23" s="0" t="n">
         <v>3958</v>
       </c>
+      <c r="C23" s="0" t="n">
+        <v>3959</v>
+      </c>
+      <c r="D23" s="0" t="n">
+        <v>3959</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="24">
       <c r="A24" s="4" t="s">
@@ -4456,6 +4550,12 @@
       <c r="B24" s="0" t="n">
         <v>466</v>
       </c>
+      <c r="C24" s="0" t="n">
+        <v>466</v>
+      </c>
+      <c r="D24" s="0" t="n">
+        <v>466</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="25">
       <c r="A25" s="4" t="s">
@@ -4464,6 +4564,12 @@
       <c r="B25" s="0" t="n">
         <v>212590</v>
       </c>
+      <c r="C25" s="0" t="n">
+        <v>212893</v>
+      </c>
+      <c r="D25" s="0" t="n">
+        <v>212718</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="26">
       <c r="A26" s="1" t="s">
@@ -4477,6 +4583,12 @@
       <c r="B27" s="0" t="n">
         <v>3353</v>
       </c>
+      <c r="C27" s="0" t="n">
+        <v>3353</v>
+      </c>
+      <c r="D27" s="0" t="n">
+        <v>3350</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="28">
       <c r="A28" s="4" t="s">
@@ -4485,6 +4597,12 @@
       <c r="B28" s="0" t="n">
         <v>131</v>
       </c>
+      <c r="C28" s="0" t="n">
+        <v>132</v>
+      </c>
+      <c r="D28" s="0" t="n">
+        <v>133</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="29">
       <c r="A29" s="4" t="s">
@@ -4493,6 +4611,12 @@
       <c r="B29" s="0" t="n">
         <v>344</v>
       </c>
+      <c r="C29" s="0" t="n">
+        <v>344</v>
+      </c>
+      <c r="D29" s="0" t="n">
+        <v>344</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="30">
       <c r="A30" s="4" t="s">
@@ -4501,6 +4625,12 @@
       <c r="B30" s="0" t="n">
         <v>351</v>
       </c>
+      <c r="C30" s="0" t="n">
+        <v>351</v>
+      </c>
+      <c r="D30" s="0" t="n">
+        <v>350</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="31">
       <c r="A31" s="4" t="s">
@@ -4509,6 +4639,12 @@
       <c r="B31" s="0" t="n">
         <v>217</v>
       </c>
+      <c r="C31" s="0" t="n">
+        <v>217</v>
+      </c>
+      <c r="D31" s="0" t="n">
+        <v>217</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="32">
       <c r="A32" s="4" t="s">
@@ -4517,6 +4653,12 @@
       <c r="B32" s="0" t="n">
         <v>671</v>
       </c>
+      <c r="C32" s="0" t="n">
+        <v>670</v>
+      </c>
+      <c r="D32" s="0" t="n">
+        <v>668</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="33">
       <c r="A33" s="1" t="s">
@@ -4530,6 +4672,12 @@
       <c r="B34" s="0" t="n">
         <v>3189</v>
       </c>
+      <c r="C34" s="0" t="n">
+        <v>3189</v>
+      </c>
+      <c r="D34" s="0" t="n">
+        <v>3188</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="35">
       <c r="A35" s="4" t="s">
@@ -4538,6 +4686,12 @@
       <c r="B35" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="C35" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D35" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="36">
       <c r="A36" s="4" t="s">
@@ -4546,6 +4700,12 @@
       <c r="B36" s="0" t="n">
         <v>337</v>
       </c>
+      <c r="C36" s="0" t="n">
+        <v>337</v>
+      </c>
+      <c r="D36" s="0" t="n">
+        <v>337</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="37">
       <c r="A37" s="4" t="s">
@@ -4554,6 +4714,12 @@
       <c r="B37" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="C37" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D37" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="38">
       <c r="A38" s="4" t="s">
@@ -4562,6 +4728,12 @@
       <c r="B38" s="0" t="n">
         <v>71</v>
       </c>
+      <c r="C38" s="0" t="n">
+        <v>71</v>
+      </c>
+      <c r="D38" s="0" t="n">
+        <v>71</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="39">
       <c r="A39" s="4" t="s">
@@ -4570,6 +4742,12 @@
       <c r="B39" s="4" t="n">
         <v>622</v>
       </c>
+      <c r="C39" s="0" t="n">
+        <v>621</v>
+      </c>
+      <c r="D39" s="0" t="n">
+        <v>620</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="40">
       <c r="A40" s="1"/>
@@ -4595,11 +4773,11 @@
       </c>
       <c r="C43" s="4" t="n">
         <f aca="false">SUM(C8:C9)</f>
-        <v>0</v>
+        <v>6161</v>
       </c>
       <c r="D43" s="4" t="n">
         <f aca="false">SUM(D8:D9)</f>
-        <v>0</v>
+        <v>6260</v>
       </c>
       <c r="E43" s="4" t="n">
         <f aca="false">SUM(E8:E9)</f>
@@ -4656,11 +4834,11 @@
       </c>
       <c r="C44" s="4" t="n">
         <f aca="false">SUM(C10:C11)</f>
-        <v>0</v>
+        <v>208</v>
       </c>
       <c r="D44" s="4" t="n">
         <f aca="false">SUM(D10:D11)</f>
-        <v>0</v>
+        <v>209</v>
       </c>
       <c r="E44" s="4" t="n">
         <f aca="false">SUM(E10:E11)</f>
@@ -4720,8 +4898,8 @@
         <v>0</v>
       </c>
       <c r="D45" s="4" t="n">
-        <f aca="false">D14</f>
-        <v>0</v>
+        <f aca="false">D18</f>
+        <v>3988</v>
       </c>
       <c r="E45" s="4" t="n">
         <f aca="false">E14</f>
@@ -4771,7 +4949,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Arial,Regular"&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Arial,Regular"Page &amp;P</oddFooter>
@@ -4994,7 +5172,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="1" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="true" usePrinterDefaults="false" verticalDpi="300"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="1" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="true" usePrinterDefaults="false" verticalDpi="300"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -5032,7 +5210,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -5068,7 +5246,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -5110,7 +5288,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>

</xml_diff>

<commit_message>
aggregated statistics for the two last releases
</commit_message>
<xml_diff>
--- a/intenz-database/src/site/resources/statistics/intenzStats-2014.xlsx
+++ b/intenz-database/src/site/resources/statistics/intenzStats-2014.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="453" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="363" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="Table" sheetId="1" state="visible" r:id="rId2"/>
@@ -133,124 +133,124 @@
   </numFmts>
   <fonts count="21">
     <font>
+      <sz val="10"/>
       <name val="Bitstream Vera Sans"/>
       <family val="2"/>
-      <sz val="10"/>
     </font>
     <font>
+      <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-      <sz val="10"/>
     </font>
     <font>
+      <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-      <sz val="10"/>
     </font>
     <font>
+      <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-      <sz val="10"/>
     </font>
     <font>
+      <b val="true"/>
+      <sz val="10"/>
       <name val="Bitstream Vera Sans"/>
       <family val="2"/>
-      <b val="true"/>
-      <sz val="10"/>
     </font>
     <font>
+      <sz val="13"/>
       <name val="Arial"/>
       <family val="2"/>
-      <sz val="13"/>
     </font>
     <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Bitstream Vera Sans"/>
       <family val="2"/>
-      <color rgb="FF000000"/>
-      <sz val="10"/>
     </font>
     <font>
+      <sz val="9"/>
       <name val="Arial"/>
       <family val="2"/>
-      <sz val="9"/>
     </font>
     <font>
+      <sz val="9.4"/>
+      <color rgb="FF000000"/>
       <name val="Bitstream Vera Sans"/>
       <family val="2"/>
-      <color rgb="FF000000"/>
-      <sz val="9.4"/>
     </font>
     <font>
+      <sz val="10.95"/>
+      <color rgb="FF000000"/>
       <name val="Bitstream Vera Sans"/>
       <family val="2"/>
-      <color rgb="FF000000"/>
-      <sz val="10.95"/>
     </font>
     <font>
+      <sz val="9.7"/>
+      <color rgb="FF000000"/>
       <name val="Bitstream Vera Sans"/>
       <family val="2"/>
-      <color rgb="FF000000"/>
-      <sz val="9.7"/>
     </font>
     <font>
+      <sz val="7.8"/>
+      <color rgb="FF000000"/>
       <name val="Bitstream Vera Sans"/>
       <family val="2"/>
-      <color rgb="FF000000"/>
-      <sz val="7.8"/>
     </font>
     <font>
+      <sz val="9.65"/>
+      <color rgb="FF000000"/>
       <name val="Bitstream Vera Sans"/>
       <family val="2"/>
-      <color rgb="FF000000"/>
-      <sz val="9.65"/>
     </font>
     <font>
+      <sz val="9.25"/>
+      <color rgb="FF000000"/>
       <name val="Bitstream Vera Sans"/>
       <family val="2"/>
-      <color rgb="FF000000"/>
-      <sz val="9.25"/>
     </font>
     <font>
+      <sz val="10.7"/>
+      <color rgb="FF000000"/>
       <name val="Bitstream Vera Sans"/>
       <family val="2"/>
-      <color rgb="FF000000"/>
-      <sz val="10.7"/>
     </font>
     <font>
+      <sz val="12.2"/>
+      <color rgb="FF000000"/>
       <name val="Bitstream Vera Sans"/>
       <family val="2"/>
-      <color rgb="FF000000"/>
-      <sz val="12.2"/>
     </font>
     <font>
+      <sz val="8.1"/>
+      <color rgb="FF000000"/>
       <name val="Bitstream Vera Sans"/>
       <family val="2"/>
-      <color rgb="FF000000"/>
-      <sz val="8.1"/>
     </font>
     <font>
+      <sz val="12.9"/>
+      <color rgb="FF000000"/>
       <name val="Bitstream Vera Sans"/>
       <family val="2"/>
-      <color rgb="FF000000"/>
-      <sz val="12.9"/>
     </font>
     <font>
+      <sz val="8.5"/>
+      <color rgb="FF000000"/>
       <name val="Bitstream Vera Sans"/>
       <family val="2"/>
-      <color rgb="FF000000"/>
-      <sz val="8.5"/>
     </font>
     <font>
+      <sz val="10.1"/>
+      <color rgb="FF000000"/>
       <name val="Bitstream Vera Sans"/>
       <family val="2"/>
-      <color rgb="FF000000"/>
-      <sz val="10.1"/>
     </font>
     <font>
+      <sz val="13.2"/>
+      <color rgb="FF000000"/>
       <name val="Bitstream Vera Sans"/>
       <family val="2"/>
-      <color rgb="FF000000"/>
-      <sz val="13.2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -397,7 +397,6 @@
   <c:lang val="en-US"/>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:tx>
         <c:rich>
           <a:bodyPr/>
@@ -413,6 +412,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -458,10 +458,10 @@
                   <c:v>97</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v/>
+                  <c:v>98</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v/>
+                  <c:v>99</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v/>
@@ -500,10 +500,10 @@
                   <c:v>5383</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v/>
+                  <c:v>5383</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v/>
+                  <c:v>5383</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v/>
@@ -566,10 +566,10 @@
                   <c:v>97</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v/>
+                  <c:v>98</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v/>
+                  <c:v>99</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v/>
@@ -608,10 +608,10 @@
                   <c:v>877</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v/>
+                  <c:v>877</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v/>
+                  <c:v>878</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v/>
@@ -674,10 +674,10 @@
                   <c:v>97</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v/>
+                  <c:v>98</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v/>
+                  <c:v>99</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v/>
@@ -716,10 +716,10 @@
                   <c:v>61</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v/>
+                  <c:v>61</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v/>
+                  <c:v>61</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v/>
@@ -782,10 +782,10 @@
                   <c:v>97</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v/>
+                  <c:v>98</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v/>
+                  <c:v>99</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v/>
@@ -824,10 +824,10 @@
                   <c:v>148</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v/>
+                  <c:v>148</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v/>
+                  <c:v>148</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v/>
@@ -890,10 +890,10 @@
                   <c:v>97</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v/>
+                  <c:v>98</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v/>
+                  <c:v>99</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v/>
@@ -935,7 +935,7 @@
                   <c:v/>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v/>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v/>
@@ -998,10 +998,10 @@
                   <c:v>97</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v/>
+                  <c:v>98</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v/>
+                  <c:v>99</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v/>
@@ -1106,10 +1106,10 @@
                   <c:v>97</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v/>
+                  <c:v>98</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v/>
+                  <c:v>99</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v/>
@@ -1151,7 +1151,7 @@
                   <c:v/>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v/>
+                  <c:v>59</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v/>
@@ -1214,10 +1214,10 @@
                   <c:v>97</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v/>
+                  <c:v>98</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v/>
+                  <c:v>99</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v/>
@@ -1283,18 +1283,19 @@
             </c:numRef>
           </c:val>
         </c:ser>
+        <c:gapWidth val="100"/>
         <c:overlap val="100"/>
-        <c:gapWidth val="100"/>
-        <c:axId val="33292058"/>
-        <c:axId val="22571829"/>
+        <c:axId val="77757444"/>
+        <c:axId val="36402019"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="33292058"/>
+        <c:axId val="77757444"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
         <c:title>
-          <c:layout/>
           <c:tx>
             <c:rich>
               <a:bodyPr/>
@@ -1310,9 +1311,8 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
         </c:title>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="low"/>
@@ -1323,20 +1323,30 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="22571829"/>
+        <c:crossAx val="36402019"/>
         <c:crossesAt val="3000"/>
+        <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
-        <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="22571829"/>
+        <c:axId val="36402019"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="3000"/>
         </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
         <c:title>
-          <c:layout/>
           <c:tx>
             <c:rich>
               <a:bodyPr/>
@@ -1357,18 +1367,8 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
         </c:title>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln>
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-        </c:majorGridlines>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1379,15 +1379,19 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="33292058"/>
+        <c:crossAx val="77757444"/>
         <c:crosses val="min"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
+        <a:ln w="12600">
+          <a:noFill/>
+        </a:ln>
       </c:spPr>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -1403,6 +1407,9 @@
     <a:solidFill>
       <a:srgbClr val="ffffff"/>
     </a:solidFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
   </c:spPr>
 </c:chartSpace>
 </file>
@@ -1412,7 +1419,6 @@
   <c:lang val="en-US"/>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:tx>
         <c:rich>
           <a:bodyPr/>
@@ -1428,6 +1434,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -1473,10 +1480,10 @@
                   <c:v>97</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v/>
+                  <c:v>98</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v/>
+                  <c:v>99</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v/>
@@ -1515,10 +1522,10 @@
                   <c:v>6260</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>6260</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>6261</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
@@ -1581,10 +1588,10 @@
                   <c:v>97</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v/>
+                  <c:v>98</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v/>
+                  <c:v>99</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v/>
@@ -1623,10 +1630,10 @@
                   <c:v>209</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>209</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>209</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
@@ -1689,10 +1696,10 @@
                   <c:v>97</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v/>
+                  <c:v>98</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v/>
+                  <c:v>99</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v/>
@@ -1734,7 +1741,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>59</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
@@ -1758,18 +1765,19 @@
             </c:numRef>
           </c:val>
         </c:ser>
+        <c:gapWidth val="100"/>
         <c:overlap val="100"/>
-        <c:gapWidth val="100"/>
-        <c:axId val="95700576"/>
-        <c:axId val="92498339"/>
+        <c:axId val="23377585"/>
+        <c:axId val="35732804"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="95700576"/>
+        <c:axId val="23377585"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
         <c:title>
-          <c:layout/>
           <c:tx>
             <c:rich>
               <a:bodyPr/>
@@ -1785,9 +1793,8 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
         </c:title>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="low"/>
@@ -1798,20 +1805,30 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="92498339"/>
+        <c:crossAx val="35732804"/>
         <c:crossesAt val="0"/>
+        <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
-        <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="92498339"/>
+        <c:axId val="35732804"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="3000"/>
         </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
         <c:title>
-          <c:layout/>
           <c:tx>
             <c:rich>
               <a:bodyPr/>
@@ -1832,18 +1849,8 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
         </c:title>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln>
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-        </c:majorGridlines>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="in"/>
         <c:tickLblPos val="nextTo"/>
@@ -1854,17 +1861,21 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="95700576"/>
+        <c:crossAx val="23377585"/>
         <c:crosses val="min"/>
         <c:majorUnit val="500"/>
         <c:minorUnit val="250"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
+        <a:ln w="12600">
+          <a:noFill/>
+        </a:ln>
       </c:spPr>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -1880,6 +1891,9 @@
     <a:solidFill>
       <a:srgbClr val="ffffff"/>
     </a:solidFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
   </c:spPr>
 </c:chartSpace>
 </file>
@@ -1889,7 +1903,6 @@
   <c:lang val="en-US"/>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:tx>
         <c:rich>
           <a:bodyPr/>
@@ -1905,6 +1918,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -1950,10 +1964,10 @@
                   <c:v>97</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v/>
+                  <c:v>98</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v/>
+                  <c:v>99</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v/>
@@ -1992,10 +2006,10 @@
                   <c:v>3350</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v/>
+                  <c:v>3350</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v/>
+                  <c:v>3349</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v/>
@@ -2058,10 +2072,10 @@
                   <c:v>97</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v/>
+                  <c:v>98</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v/>
+                  <c:v>99</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v/>
@@ -2100,10 +2114,10 @@
                   <c:v>133</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v/>
+                  <c:v>133</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v/>
+                  <c:v>136</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v/>
@@ -2166,10 +2180,10 @@
                   <c:v>97</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v/>
+                  <c:v>98</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v/>
+                  <c:v>99</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v/>
@@ -2208,10 +2222,10 @@
                   <c:v>344</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v/>
+                  <c:v>344</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v/>
+                  <c:v>344</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v/>
@@ -2274,10 +2288,10 @@
                   <c:v>97</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v/>
+                  <c:v>98</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v/>
+                  <c:v>99</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v/>
@@ -2316,10 +2330,10 @@
                   <c:v>350</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v/>
+                  <c:v>350</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v/>
+                  <c:v>350</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v/>
@@ -2382,10 +2396,10 @@
                   <c:v>97</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v/>
+                  <c:v>98</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v/>
+                  <c:v>99</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v/>
@@ -2424,10 +2438,10 @@
                   <c:v>217</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v/>
+                  <c:v>217</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v/>
+                  <c:v>217</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v/>
@@ -2490,10 +2504,10 @@
                   <c:v>97</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v/>
+                  <c:v>98</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v/>
+                  <c:v>99</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v/>
@@ -2532,10 +2546,10 @@
                   <c:v>668</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v/>
+                  <c:v>668</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v/>
+                  <c:v>665</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v/>
@@ -2559,18 +2573,19 @@
             </c:numRef>
           </c:val>
         </c:ser>
+        <c:gapWidth val="100"/>
         <c:overlap val="100"/>
-        <c:gapWidth val="100"/>
-        <c:axId val="9211191"/>
-        <c:axId val="74735576"/>
+        <c:axId val="33603714"/>
+        <c:axId val="53699372"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="9211191"/>
+        <c:axId val="33603714"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
         <c:title>
-          <c:layout/>
           <c:tx>
             <c:rich>
               <a:bodyPr/>
@@ -2591,9 +2606,8 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
         </c:title>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="low"/>
@@ -2604,19 +2618,29 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="74735576"/>
+        <c:crossAx val="53699372"/>
         <c:crossesAt val="0"/>
+        <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
-        <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="74735576"/>
+        <c:axId val="53699372"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
         <c:title>
-          <c:layout/>
           <c:tx>
             <c:rich>
               <a:bodyPr/>
@@ -2637,18 +2661,8 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
         </c:title>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln>
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-        </c:majorGridlines>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2659,15 +2673,19 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="9211191"/>
+        <c:crossAx val="33603714"/>
         <c:crosses val="min"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
+        <a:ln w="12600">
+          <a:noFill/>
+        </a:ln>
       </c:spPr>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -2683,6 +2701,9 @@
     <a:solidFill>
       <a:srgbClr val="ffffff"/>
     </a:solidFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
   </c:spPr>
 </c:chartSpace>
 </file>
@@ -2692,7 +2713,6 @@
   <c:lang val="en-US"/>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:tx>
         <c:rich>
           <a:bodyPr/>
@@ -2708,6 +2728,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -2753,10 +2774,10 @@
                   <c:v>97</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v/>
+                  <c:v>98</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v/>
+                  <c:v>99</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v/>
@@ -2795,10 +2816,10 @@
                   <c:v>212718</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v/>
+                  <c:v>213421</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v/>
+                  <c:v>216354</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v/>
@@ -2861,10 +2882,10 @@
                   <c:v>97</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v/>
+                  <c:v>98</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v/>
+                  <c:v>99</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v/>
@@ -2903,10 +2924,10 @@
                   <c:v>466</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v/>
+                  <c:v>466</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v/>
+                  <c:v>466</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v/>
@@ -2969,10 +2990,10 @@
                   <c:v>97</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v/>
+                  <c:v>98</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v/>
+                  <c:v>99</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v/>
@@ -3011,10 +3032,10 @@
                   <c:v>3959</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v/>
+                  <c:v>3959</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v/>
+                  <c:v>3956</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v/>
@@ -3077,10 +3098,10 @@
                   <c:v>97</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v/>
+                  <c:v>98</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v/>
+                  <c:v>99</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v/>
@@ -3119,10 +3140,10 @@
                   <c:v>573</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v/>
+                  <c:v>573</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v/>
+                  <c:v>575</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v/>
@@ -3146,13 +3167,13 @@
             </c:numRef>
           </c:val>
         </c:ser>
+        <c:gapWidth val="100"/>
         <c:overlap val="100"/>
-        <c:gapWidth val="100"/>
-        <c:axId val="92360204"/>
-        <c:axId val="39946026"/>
+        <c:axId val="12290129"/>
+        <c:axId val="89860436"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="92360204"/>
+        <c:axId val="12290129"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3168,20 +3189,30 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="39946026"/>
+        <c:crossAx val="89860436"/>
         <c:crossesAt val="0"/>
+        <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
-        <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="39946026"/>
+        <c:axId val="89860436"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="160000"/>
         </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
         <c:title>
-          <c:layout/>
           <c:tx>
             <c:rich>
               <a:bodyPr/>
@@ -3202,18 +3233,8 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
         </c:title>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln>
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-        </c:majorGridlines>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -3224,15 +3245,19 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="92360204"/>
+        <c:crossAx val="12290129"/>
         <c:crosses val="min"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
+        <a:ln w="12600">
+          <a:noFill/>
+        </a:ln>
       </c:spPr>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -3248,6 +3273,9 @@
     <a:solidFill>
       <a:srgbClr val="ffffff"/>
     </a:solidFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
   </c:spPr>
 </c:chartSpace>
 </file>
@@ -3257,7 +3285,6 @@
   <c:lang val="en-US"/>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:tx>
         <c:rich>
           <a:bodyPr/>
@@ -3273,6 +3300,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -3318,10 +3346,10 @@
                   <c:v>97</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v/>
+                  <c:v>98</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v/>
+                  <c:v>99</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v/>
@@ -3360,10 +3388,10 @@
                   <c:v>224291</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v/>
+                  <c:v>225002</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v/>
+                  <c:v>228051</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v/>
@@ -3426,10 +3454,10 @@
                   <c:v>97</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v/>
+                  <c:v>98</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v/>
+                  <c:v>99</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v/>
@@ -3468,10 +3496,10 @@
                   <c:v>1440</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v/>
+                  <c:v>1440</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v/>
+                  <c:v>1440</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v/>
@@ -3534,10 +3562,10 @@
                   <c:v>97</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v/>
+                  <c:v>98</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v/>
+                  <c:v>99</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v/>
@@ -3576,10 +3604,10 @@
                   <c:v>3988</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v/>
+                  <c:v>3988</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v/>
+                  <c:v>3985</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v/>
@@ -3642,10 +3670,10 @@
                   <c:v>97</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v/>
+                  <c:v>98</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v/>
+                  <c:v>99</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v/>
@@ -3684,10 +3712,10 @@
                   <c:v>1747</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v/>
+                  <c:v>1747</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v/>
+                  <c:v>1749</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v/>
@@ -3711,13 +3739,13 @@
             </c:numRef>
           </c:val>
         </c:ser>
+        <c:gapWidth val="100"/>
         <c:overlap val="100"/>
-        <c:gapWidth val="100"/>
-        <c:axId val="91548494"/>
-        <c:axId val="53736695"/>
+        <c:axId val="28534543"/>
+        <c:axId val="91210920"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="91548494"/>
+        <c:axId val="28534543"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3733,20 +3761,30 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="53736695"/>
+        <c:crossAx val="91210920"/>
         <c:crossesAt val="0"/>
+        <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
-        <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="53736695"/>
+        <c:axId val="91210920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="160000"/>
         </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
         <c:title>
-          <c:layout/>
           <c:tx>
             <c:rich>
               <a:bodyPr/>
@@ -3767,18 +3805,8 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
         </c:title>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln>
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-        </c:majorGridlines>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -3789,15 +3817,19 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="91548494"/>
+        <c:crossAx val="28534543"/>
         <c:crosses val="min"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
+        <a:ln w="12600">
+          <a:noFill/>
+        </a:ln>
       </c:spPr>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -3813,6 +3845,9 @@
     <a:solidFill>
       <a:srgbClr val="ffffff"/>
     </a:solidFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
   </c:spPr>
 </c:chartSpace>
 </file>
@@ -3842,6 +3877,118 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="5"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="6"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="7"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="8"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="9"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="10"/>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
               <c:f>Table!$B$1:$L$1</c:f>
@@ -3857,10 +4004,10 @@
                   <c:v>97</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v/>
+                  <c:v>98</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v/>
+                  <c:v>99</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v/>
@@ -3899,10 +4046,10 @@
                   <c:v>20319</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v/>
+                  <c:v>20318</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v/>
+                  <c:v>20343</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v/>
@@ -3927,16 +4074,17 @@
           </c:val>
         </c:ser>
         <c:marker val="0"/>
-        <c:axId val="31180946"/>
-        <c:axId val="65128132"/>
+        <c:axId val="42885817"/>
+        <c:axId val="96584395"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="31180946"/>
+        <c:axId val="42885817"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
         <c:title>
-          <c:layout/>
           <c:tx>
             <c:rich>
               <a:bodyPr/>
@@ -3957,9 +4105,8 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
         </c:title>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="low"/>
@@ -3970,20 +4117,30 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="65128132"/>
+        <c:crossAx val="96584395"/>
         <c:crossesAt val="17000"/>
+        <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
-        <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="65128132"/>
+        <c:axId val="96584395"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
         </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
         <c:title>
-          <c:layout/>
           <c:tx>
             <c:rich>
               <a:bodyPr/>
@@ -4004,18 +4161,8 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
         </c:title>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln>
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-        </c:majorGridlines>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -4026,13 +4173,16 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="31180946"/>
+        <c:crossAx val="42885817"/>
         <c:crosses val="min"/>
       </c:valAx>
       <c:spPr>
         <a:solidFill>
           <a:srgbClr val="d9d9d9"/>
         </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
       </c:spPr>
     </c:plotArea>
     <c:plotVisOnly val="1"/>
@@ -4041,6 +4191,9 @@
     <a:solidFill>
       <a:srgbClr val="ffffff"/>
     </a:solidFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
   </c:spPr>
 </c:chartSpace>
 </file>
@@ -4052,13 +4205,13 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>165600</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>4320</xdr:rowOff>
+      <xdr:rowOff>5040</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>93600</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>3240</xdr:rowOff>
+      <xdr:rowOff>3600</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4066,8 +4219,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="165600" y="163440"/>
-        <a:ext cx="11599920" cy="3833640"/>
+        <a:off x="165600" y="164160"/>
+        <a:ext cx="11599920" cy="3833280"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4082,13 +4235,13 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>152280</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>91080</xdr:rowOff>
+      <xdr:rowOff>91800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>119160</xdr:colOff>
       <xdr:row>49</xdr:row>
-      <xdr:rowOff>3240</xdr:rowOff>
+      <xdr:rowOff>3600</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4096,8 +4249,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="152280" y="4084920"/>
-        <a:ext cx="11638800" cy="3737520"/>
+        <a:off x="152280" y="4085640"/>
+        <a:ext cx="11638800" cy="3737160"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4123,7 +4276,7 @@
       <xdr:col>14</xdr:col>
       <xdr:colOff>678600</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>11520</xdr:rowOff>
+      <xdr:rowOff>11880</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4132,7 +4285,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="56160"/>
-        <a:ext cx="11962440" cy="3803760"/>
+        <a:ext cx="11962440" cy="3804120"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4156,9 +4309,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>491760</xdr:colOff>
+      <xdr:colOff>492120</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>144000</xdr:rowOff>
+      <xdr:rowOff>144360</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4167,7 +4320,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="292680" y="19440"/>
-        <a:ext cx="11245320" cy="3661200"/>
+        <a:ext cx="11245680" cy="3661560"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4182,11 +4335,11 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>318600</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>150480</xdr:rowOff>
+      <xdr:rowOff>151200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>522000</xdr:colOff>
+      <xdr:colOff>522360</xdr:colOff>
       <xdr:row>47</xdr:row>
       <xdr:rowOff>91080</xdr:rowOff>
     </xdr:to>
@@ -4196,8 +4349,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="318600" y="3846600"/>
-        <a:ext cx="11249640" cy="3765960"/>
+        <a:off x="318600" y="3847320"/>
+        <a:ext cx="11250000" cy="3765240"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4221,9 +4374,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>82800</xdr:colOff>
+      <xdr:colOff>83160</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>88920</xdr:rowOff>
+      <xdr:rowOff>89280</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4232,7 +4385,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="59400" y="51840"/>
-        <a:ext cx="10975680" cy="3893760"/>
+        <a:ext cx="10976040" cy="3894120"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4253,7 +4406,7 @@
   <dimension ref="A1:O45"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="E1" activeCellId="0" pane="topLeft" sqref="E1"/>
+      <selection activeCell="G1" activeCellId="0" pane="topLeft" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.1"/>
@@ -4275,6 +4428,14 @@
       <c r="D1" s="1" t="n">
         <v>97</v>
       </c>
+      <c r="E1" s="1" t="n">
+        <v>98</v>
+      </c>
+      <c r="F1" s="1" t="n">
+        <v>99</v>
+      </c>
+      <c r="G1" s="0"/>
+      <c r="H1" s="0"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="2">
       <c r="A2" s="1" t="s">
@@ -4289,10 +4450,12 @@
       <c r="D2" s="2" t="n">
         <v>41704</v>
       </c>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
+      <c r="E2" s="2" t="n">
+        <v>41738</v>
+      </c>
+      <c r="F2" s="2" t="n">
+        <v>41815</v>
+      </c>
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
@@ -4314,6 +4477,12 @@
       <c r="D3" s="0" t="n">
         <v>6</v>
       </c>
+      <c r="E3" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="F3" s="0" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="4">
       <c r="A4" s="1" t="s">
@@ -4328,6 +4497,12 @@
       <c r="D4" s="0" t="n">
         <v>69</v>
       </c>
+      <c r="E4" s="0" t="n">
+        <v>69</v>
+      </c>
+      <c r="F4" s="0" t="n">
+        <v>69</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="5">
       <c r="A5" s="1" t="s">
@@ -4342,7 +4517,12 @@
       <c r="D5" s="0" t="n">
         <v>287</v>
       </c>
-      <c r="H5" s="3"/>
+      <c r="E5" s="0" t="n">
+        <v>287</v>
+      </c>
+      <c r="F5" s="0" t="n">
+        <v>288</v>
+      </c>
       <c r="I5" s="3"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="6">
@@ -4358,7 +4538,12 @@
       <c r="D6" s="0" t="n">
         <v>20319</v>
       </c>
-      <c r="H6" s="3"/>
+      <c r="E6" s="0" t="n">
+        <v>20318</v>
+      </c>
+      <c r="F6" s="0" t="n">
+        <v>20343</v>
+      </c>
       <c r="I6" s="3"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="7">
@@ -4366,7 +4551,6 @@
         <v>6</v>
       </c>
       <c r="B7" s="4"/>
-      <c r="H7" s="3"/>
       <c r="I7" s="3"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="8">
@@ -4382,7 +4566,12 @@
       <c r="D8" s="0" t="n">
         <v>5383</v>
       </c>
-      <c r="H8" s="3"/>
+      <c r="E8" s="0" t="n">
+        <v>5383</v>
+      </c>
+      <c r="F8" s="0" t="n">
+        <v>5383</v>
+      </c>
       <c r="I8" s="3"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="9">
@@ -4398,6 +4587,12 @@
       <c r="D9" s="0" t="n">
         <v>877</v>
       </c>
+      <c r="E9" s="0" t="n">
+        <v>877</v>
+      </c>
+      <c r="F9" s="0" t="n">
+        <v>878</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="10">
       <c r="A10" s="4" t="s">
@@ -4412,6 +4607,12 @@
       <c r="D10" s="0" t="n">
         <v>61</v>
       </c>
+      <c r="E10" s="0" t="n">
+        <v>61</v>
+      </c>
+      <c r="F10" s="0" t="n">
+        <v>61</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="11">
       <c r="A11" s="4" t="s">
@@ -4426,12 +4627,21 @@
       <c r="D11" s="0" t="n">
         <v>148</v>
       </c>
+      <c r="E11" s="0" t="n">
+        <v>148</v>
+      </c>
+      <c r="F11" s="0" t="n">
+        <v>148</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="12">
       <c r="A12" s="4" t="s">
         <v>11</v>
       </c>
       <c r="B12" s="4"/>
+      <c r="F12" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="13">
       <c r="A13" s="4" t="s">
@@ -4443,13 +4653,16 @@
         <v>13</v>
       </c>
       <c r="B14" s="4"/>
+      <c r="F14" s="0" t="n">
+        <v>59</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="15">
       <c r="A15" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="16">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="16">
       <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
@@ -4467,6 +4680,12 @@
       <c r="D17" s="0" t="n">
         <v>1747</v>
       </c>
+      <c r="E17" s="0" t="n">
+        <v>1747</v>
+      </c>
+      <c r="F17" s="0" t="n">
+        <v>1749</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="18">
       <c r="A18" s="4" t="s">
@@ -4481,6 +4700,12 @@
       <c r="D18" s="0" t="n">
         <v>3988</v>
       </c>
+      <c r="E18" s="0" t="n">
+        <v>3988</v>
+      </c>
+      <c r="F18" s="0" t="n">
+        <v>3985</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="19">
       <c r="A19" s="4" t="s">
@@ -4495,8 +4720,14 @@
       <c r="D19" s="0" t="n">
         <v>1440</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="20">
+      <c r="E19" s="0" t="n">
+        <v>1440</v>
+      </c>
+      <c r="F19" s="0" t="n">
+        <v>1440</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="20">
       <c r="A20" s="4" t="s">
         <v>19</v>
       </c>
@@ -4509,8 +4740,14 @@
       <c r="D20" s="0" t="n">
         <v>224291</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="21">
+      <c r="E20" s="0" t="n">
+        <v>225002</v>
+      </c>
+      <c r="F20" s="0" t="n">
+        <v>228051</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="21">
       <c r="A21" s="1" t="s">
         <v>20</v>
       </c>
@@ -4528,6 +4765,12 @@
       <c r="D22" s="0" t="n">
         <v>573</v>
       </c>
+      <c r="E22" s="0" t="n">
+        <v>573</v>
+      </c>
+      <c r="F22" s="0" t="n">
+        <v>575</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="23">
       <c r="A23" s="4" t="s">
@@ -4542,6 +4785,12 @@
       <c r="D23" s="0" t="n">
         <v>3959</v>
       </c>
+      <c r="E23" s="0" t="n">
+        <v>3959</v>
+      </c>
+      <c r="F23" s="0" t="n">
+        <v>3956</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="24">
       <c r="A24" s="4" t="s">
@@ -4556,8 +4805,14 @@
       <c r="D24" s="0" t="n">
         <v>466</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="25">
+      <c r="E24" s="0" t="n">
+        <v>466</v>
+      </c>
+      <c r="F24" s="0" t="n">
+        <v>466</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="25">
       <c r="A25" s="4" t="s">
         <v>19</v>
       </c>
@@ -4569,6 +4824,12 @@
       </c>
       <c r="D25" s="0" t="n">
         <v>212718</v>
+      </c>
+      <c r="E25" s="0" t="n">
+        <v>213421</v>
+      </c>
+      <c r="F25" s="0" t="n">
+        <v>216354</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="26">
@@ -4589,6 +4850,12 @@
       <c r="D27" s="0" t="n">
         <v>3350</v>
       </c>
+      <c r="E27" s="0" t="n">
+        <v>3350</v>
+      </c>
+      <c r="F27" s="0" t="n">
+        <v>3349</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="28">
       <c r="A28" s="4" t="s">
@@ -4603,6 +4870,12 @@
       <c r="D28" s="0" t="n">
         <v>133</v>
       </c>
+      <c r="E28" s="0" t="n">
+        <v>133</v>
+      </c>
+      <c r="F28" s="0" t="n">
+        <v>136</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="29">
       <c r="A29" s="4" t="s">
@@ -4617,6 +4890,12 @@
       <c r="D29" s="0" t="n">
         <v>344</v>
       </c>
+      <c r="E29" s="0" t="n">
+        <v>344</v>
+      </c>
+      <c r="F29" s="0" t="n">
+        <v>344</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="30">
       <c r="A30" s="4" t="s">
@@ -4631,6 +4910,12 @@
       <c r="D30" s="0" t="n">
         <v>350</v>
       </c>
+      <c r="E30" s="0" t="n">
+        <v>350</v>
+      </c>
+      <c r="F30" s="0" t="n">
+        <v>350</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="31">
       <c r="A31" s="4" t="s">
@@ -4645,6 +4930,12 @@
       <c r="D31" s="0" t="n">
         <v>217</v>
       </c>
+      <c r="E31" s="0" t="n">
+        <v>217</v>
+      </c>
+      <c r="F31" s="0" t="n">
+        <v>217</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="32">
       <c r="A32" s="4" t="s">
@@ -4659,6 +4950,12 @@
       <c r="D32" s="0" t="n">
         <v>668</v>
       </c>
+      <c r="E32" s="0" t="n">
+        <v>668</v>
+      </c>
+      <c r="F32" s="0" t="n">
+        <v>665</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="33">
       <c r="A33" s="1" t="s">
@@ -4678,6 +4975,12 @@
       <c r="D34" s="0" t="n">
         <v>3188</v>
       </c>
+      <c r="E34" s="0" t="n">
+        <v>3188</v>
+      </c>
+      <c r="F34" s="0" t="n">
+        <v>3188</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="35">
       <c r="A35" s="4" t="s">
@@ -4692,6 +4995,12 @@
       <c r="D35" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="E35" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F35" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="36">
       <c r="A36" s="4" t="s">
@@ -4706,6 +5015,12 @@
       <c r="D36" s="0" t="n">
         <v>337</v>
       </c>
+      <c r="E36" s="0" t="n">
+        <v>337</v>
+      </c>
+      <c r="F36" s="0" t="n">
+        <v>337</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="37">
       <c r="A37" s="4" t="s">
@@ -4720,6 +5035,12 @@
       <c r="D37" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="E37" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F37" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="38">
       <c r="A38" s="4" t="s">
@@ -4734,6 +5055,12 @@
       <c r="D38" s="0" t="n">
         <v>71</v>
       </c>
+      <c r="E38" s="0" t="n">
+        <v>71</v>
+      </c>
+      <c r="F38" s="0" t="n">
+        <v>70</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="39">
       <c r="A39" s="4" t="s">
@@ -4748,6 +5075,12 @@
       <c r="D39" s="0" t="n">
         <v>620</v>
       </c>
+      <c r="E39" s="0" t="n">
+        <v>620</v>
+      </c>
+      <c r="F39" s="0" t="n">
+        <v>617</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="40">
       <c r="A40" s="1"/>
@@ -4781,11 +5114,11 @@
       </c>
       <c r="E43" s="4" t="n">
         <f aca="false">SUM(E8:E9)</f>
-        <v>0</v>
+        <v>6260</v>
       </c>
       <c r="F43" s="4" t="n">
         <f aca="false">SUM(F8:F9)</f>
-        <v>0</v>
+        <v>6261</v>
       </c>
       <c r="G43" s="4" t="n">
         <f aca="false">SUM(G8:G9)</f>
@@ -4842,11 +5175,11 @@
       </c>
       <c r="E44" s="4" t="n">
         <f aca="false">SUM(E10:E11)</f>
-        <v>0</v>
+        <v>209</v>
       </c>
       <c r="F44" s="4" t="n">
         <f aca="false">SUM(F10:F11)</f>
-        <v>0</v>
+        <v>209</v>
       </c>
       <c r="G44" s="4" t="n">
         <f aca="false">SUM(G10:G11)</f>
@@ -4907,7 +5240,7 @@
       </c>
       <c r="F45" s="4" t="n">
         <f aca="false">F14</f>
-        <v>0</v>
+        <v>59</v>
       </c>
       <c r="G45" s="4" t="n">
         <f aca="false">G14</f>
@@ -4949,7 +5282,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Arial,Regular"&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Arial,Regular"Page &amp;P</oddFooter>
@@ -5172,7 +5505,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="1" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="true" usePrinterDefaults="false" verticalDpi="300"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="1" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="true" usePrinterDefaults="false" verticalDpi="300"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -5210,7 +5543,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -5246,7 +5579,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -5288,7 +5621,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>

</xml_diff>